<commit_message>
KIBON-603: Pivot Tabellen angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag_DE.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag_DE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/medu/dev/ebegu/ebegu-server/src/main/resources/reporting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egch\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2AB7BF-CA99-5E44-BBCE-346CAAEAFCA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E616B68A-8700-4483-8A3F-4086EDE12802}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -94,16 +94,16 @@
     <t>Values</t>
   </si>
   <si>
-    <t>Offene Beschwerden</t>
-  </si>
-  <si>
     <t>Offene Mahnungen</t>
   </si>
   <si>
     <t>Nicht freigegebene Gesuche</t>
   </si>
   <si>
-    <t>(All)</t>
+    <t>(Alle)</t>
+  </si>
+  <si>
+    <t>Offene Beschwerde</t>
   </si>
 </sst>
 </file>
@@ -176,20 +176,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <border>
         <left style="thin">
@@ -259,6 +248,17 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="1"/>
@@ -327,6 +327,17 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="1"/>
@@ -395,6 +406,17 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="1"/>
@@ -463,28 +485,15 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -529,6 +538,41 @@
           <color theme="1"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -544,7 +588,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Menzies Duncan" refreshedDate="43532.499186921297" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Egli Christian" refreshedDate="43641.381379976854" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
@@ -608,7 +652,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B4:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" compact="0" showAll="0">
@@ -666,21 +710,21 @@
     <pageField fld="4" hier="-1"/>
   </pageFields>
   <dataFields count="3">
-    <dataField name="Nicht freigegebene Gesuche" fld="6" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Offene Mahnungen" fld="7" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Offene Beschwerden" fld="8" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Nicht freigegebene Gesuche" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Offene Mahnungen" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Offene Beschwerde" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="30">
+    <format dxfId="21">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="23">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -691,10 +735,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="25">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -705,7 +749,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="27">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
   </formats>
@@ -719,7 +763,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -761,7 +805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -813,7 +857,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1019,45 +1063,46 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
@@ -1066,7 +1111,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1074,43 +1119,43 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1125,20 +1170,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>

</xml_diff>